<commit_message>
add exception handling for file upload
</commit_message>
<xml_diff>
--- a/test_data.xlsx
+++ b/test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/panyong/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ECE63C6-B6F2-C747-A644-65B6AF36BEC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B3BADF-F83A-B747-BDDE-9302B8022450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="660" windowWidth="28040" windowHeight="17440" xr2:uid="{D0D5140B-E773-B94B-B14F-41E0C43F919D}"/>
+    <workbookView xWindow="2200" yWindow="760" windowWidth="28040" windowHeight="17440" xr2:uid="{D0D5140B-E773-B94B-B14F-41E0C43F919D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,19 +38,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>Old town white coffee</t>
+  </si>
+  <si>
     <t>Description</t>
   </si>
   <si>
-    <t>red paper bag</t>
+    <t>red bag</t>
   </si>
   <si>
-    <t>coffee powder</t>
-  </si>
-  <si>
-    <t>metal sheet</t>
-  </si>
-  <si>
-    <t>No.</t>
+    <t>metal plate</t>
   </si>
 </sst>
 </file>
@@ -425,7 +425,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -435,10 +435,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -446,7 +446,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -454,7 +454,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -462,7 +462,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>